<commit_message>
Changes made as of 21 September
rearranged folder structure and added new folders.
</commit_message>
<xml_diff>
--- a/ContactsMatrix.xlsx
+++ b/ContactsMatrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="84" windowWidth="22980" windowHeight="6624" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="84" windowWidth="22980" windowHeight="6624"/>
   </bookViews>
   <sheets>
     <sheet name="ContactInfo" sheetId="1" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>M(All day), Tu(&gt;3pm),  Wed(1-6pm), Th(&gt;3pm), Sat(All day)</t>
   </si>
   <si>
-    <t>Xintong Shi (Steven)</t>
-  </si>
-  <si>
     <t>248-701-8587</t>
   </si>
   <si>
@@ -430,6 +427,9 @@
   </si>
   <si>
     <t>Blue, Purple, Gray, Red,Yellow, Green</t>
+  </si>
+  <si>
+    <t>Xinfeng Shi (Steven)</t>
   </si>
 </sst>
 </file>
@@ -732,6 +732,48 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -744,15 +786,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -771,44 +804,11 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1114,8 +1114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1142,13 +1142,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1162,16 +1162,16 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" t="s">
         <v>130</v>
       </c>
-      <c r="F2" t="s">
-        <v>131</v>
-      </c>
       <c r="G2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1188,13 +1188,13 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1211,13 +1211,13 @@
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1234,82 +1234,82 @@
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="s">
-        <v>27</v>
-      </c>
       <c r="E7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F8" t="s">
+        <v>136</v>
+      </c>
+      <c r="G8" t="s">
         <v>83</v>
-      </c>
-      <c r="B8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" t="s">
-        <v>126</v>
-      </c>
-      <c r="F8" t="s">
-        <v>137</v>
-      </c>
-      <c r="G8" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1333,7 +1333,7 @@
   </sheetPr>
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29:E34"/>
     </sheetView>
   </sheetViews>
@@ -1354,39 +1354,39 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>34</v>
-      </c>
       <c r="H1" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J1" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="12" t="s">
         <v>77</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1396,512 +1396,507 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="J2" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" s="44" t="s">
-        <v>94</v>
-      </c>
-      <c r="F3" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="H3" s="38" t="s">
-        <v>99</v>
+        <v>36</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>98</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="38"/>
+        <v>37</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="26"/>
       <c r="J4" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="38"/>
+        <v>38</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="26"/>
       <c r="J5" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="38"/>
+        <v>39</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="26"/>
       <c r="J6" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="K6" s="19" t="s">
         <v>117</v>
-      </c>
-      <c r="K6" s="19" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="38"/>
+        <v>40</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" s="48"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="26"/>
       <c r="J7" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="K7" s="20" t="s">
         <v>119</v>
-      </c>
-      <c r="K7" s="20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="38"/>
+        <v>41</v>
+      </c>
+      <c r="B8" s="31"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="26"/>
       <c r="J8" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="K8" s="21" t="s">
         <v>121</v>
-      </c>
-      <c r="K8" s="21" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="38"/>
+        <v>42</v>
+      </c>
+      <c r="B9" s="31"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="38"/>
+        <v>43</v>
+      </c>
+      <c r="B10" s="31"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="47"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="37" t="s">
-        <v>108</v>
+        <v>44</v>
+      </c>
+      <c r="B11" s="31"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="33" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="37"/>
+        <v>45</v>
+      </c>
+      <c r="B12" s="31"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="33"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="47"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="E13" s="45"/>
-      <c r="F13" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="37"/>
+        <v>46</v>
+      </c>
+      <c r="B13" s="31"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="48"/>
+      <c r="F13" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="G13" s="45"/>
+      <c r="H13" s="33"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="37"/>
+        <v>47</v>
+      </c>
+      <c r="B14" s="31"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="33"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="47"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="G15" s="34"/>
-      <c r="H15" s="36" t="s">
-        <v>109</v>
+        <v>48</v>
+      </c>
+      <c r="B15" s="31"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="G15" s="45"/>
+      <c r="H15" s="32" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="36"/>
+        <v>49</v>
+      </c>
+      <c r="B16" s="31"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="G17" s="34"/>
-      <c r="H17" s="36"/>
+        <v>103</v>
+      </c>
+      <c r="G17" s="45"/>
+      <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="38" t="s">
-        <v>71</v>
+        <v>51</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>70</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="G18" s="34"/>
-      <c r="H18" s="36"/>
+        <v>73</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="G18" s="45"/>
+      <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="D19" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" s="42" t="s">
-        <v>96</v>
-      </c>
-      <c r="F19" s="28"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="36"/>
+        <v>52</v>
+      </c>
+      <c r="B19" s="26"/>
+      <c r="C19" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" s="35"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="32"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="36"/>
+        <v>53</v>
+      </c>
+      <c r="B20" s="26"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="32"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="38"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="36"/>
+        <v>54</v>
+      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="32"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" s="38"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="46" t="s">
-        <v>97</v>
-      </c>
-      <c r="F22" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="G22" s="34"/>
-      <c r="H22" s="36"/>
+        <v>55</v>
+      </c>
+      <c r="B22" s="26"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="G22" s="45"/>
+      <c r="H22" s="32"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="E23" s="42"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="36"/>
+        <v>56</v>
+      </c>
+      <c r="B23" s="26"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="29"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="32"/>
     </row>
     <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="38"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="36"/>
+        <v>57</v>
+      </c>
+      <c r="B24" s="26"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="32"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="36"/>
+        <v>58</v>
+      </c>
+      <c r="B25" s="26"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="32"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="38"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="36"/>
+        <v>59</v>
+      </c>
+      <c r="B26" s="26"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="32"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="F27" s="28"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="36"/>
+        <v>60</v>
+      </c>
+      <c r="B27" s="26"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="F27" s="35"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="32"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="36"/>
+        <v>61</v>
+      </c>
+      <c r="B28" s="26"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="32"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="F29" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="G29" s="34"/>
-      <c r="H29" s="39" t="s">
-        <v>108</v>
+        <v>62</v>
+      </c>
+      <c r="B29" s="26"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="F29" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="G29" s="45"/>
+      <c r="H29" s="23" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" s="40"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="40"/>
+        <v>63</v>
+      </c>
+      <c r="B30" s="26"/>
+      <c r="C30" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="24"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="24"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="40"/>
+        <v>64</v>
+      </c>
+      <c r="B31" s="26"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="24"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" s="38"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="40"/>
+        <v>65</v>
+      </c>
+      <c r="B32" s="26"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="24"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="40"/>
+        <v>66</v>
+      </c>
+      <c r="B33" s="26"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="24"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B34" s="38"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="41"/>
+        <v>67</v>
+      </c>
+      <c r="B34" s="26"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="D7:D12"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="B18:B34"/>
-    <mergeCell ref="C3:C16"/>
-    <mergeCell ref="D23:D34"/>
-    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="G3:G34"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="E3:E16"/>
     <mergeCell ref="E22:E26"/>
     <mergeCell ref="B7:B16"/>
     <mergeCell ref="B3:B6"/>
@@ -1918,9 +1913,14 @@
     <mergeCell ref="E29:E34"/>
     <mergeCell ref="F22:F28"/>
     <mergeCell ref="F29:F34"/>
-    <mergeCell ref="G3:G34"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="E3:E16"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="D7:D12"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="B18:B34"/>
+    <mergeCell ref="C3:C16"/>
+    <mergeCell ref="D23:D34"/>
+    <mergeCell ref="D13:D16"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>

</xml_diff>